<commit_message>
- updated journal - added optimize instrument - calculated dark correction
</commit_message>
<xml_diff>
--- a/doc/journal/Arbeitsjournal.xlsx
+++ b/doc/journal/Arbeitsjournal.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andreas\Documents\Projects\Spektrometer\portableSpectrometer\doc\journal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Andreas/Projects/Bachelorthesis/portableSpectrometer/doc/journal/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="16800" windowHeight="19515" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="19520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Arbeitsjournal" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="Andreas Lüscher" sheetId="5" r:id="rId3"/>
     <sheet name="Zusatz" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="94">
   <si>
     <t>Arbeitsjournal Übersicht</t>
   </si>
@@ -303,12 +303,21 @@
   </si>
   <si>
     <t>Demo Einrichtung</t>
+  </si>
+  <si>
+    <t>Prototyp 2</t>
+  </si>
+  <si>
+    <t>Optimize Instrument</t>
+  </si>
+  <si>
+    <t>Dark correction</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -458,7 +467,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -474,9 +483,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="de-CH"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -518,6 +527,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -578,79 +588,79 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>39</c:v>
+                  <c:v>39.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>40.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41</c:v>
+                  <c:v>41.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42</c:v>
+                  <c:v>42.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43</c:v>
+                  <c:v>43.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44</c:v>
+                  <c:v>44.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>45</c:v>
+                  <c:v>45.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>46</c:v>
+                  <c:v>46.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>47</c:v>
+                  <c:v>47.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>48</c:v>
+                  <c:v>48.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>49</c:v>
+                  <c:v>49.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>50</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>51</c:v>
+                  <c:v>51.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>52</c:v>
+                  <c:v>52.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>9</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -662,85 +672,85 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40</c:v>
+                  <c:v>40.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>56</c:v>
+                  <c:v>56.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>72</c:v>
+                  <c:v>72.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>88</c:v>
+                  <c:v>88.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>104</c:v>
+                  <c:v>104.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>120</c:v>
+                  <c:v>120.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>136</c:v>
+                  <c:v>136.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>152</c:v>
+                  <c:v>152.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>168</c:v>
+                  <c:v>168.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>184</c:v>
+                  <c:v>184.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>200</c:v>
+                  <c:v>200.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>200</c:v>
+                  <c:v>200.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>200</c:v>
+                  <c:v>200.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>216</c:v>
+                  <c:v>216.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>232</c:v>
+                  <c:v>232.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>248</c:v>
+                  <c:v>248.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>264</c:v>
+                  <c:v>264.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>280</c:v>
+                  <c:v>280.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>296</c:v>
+                  <c:v>296.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>312</c:v>
+                  <c:v>312.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>328</c:v>
+                  <c:v>328.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>344</c:v>
+                  <c:v>344.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>360</c:v>
+                  <c:v>360.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-8D59-4CCE-98CB-8B5DAB46F197}"/>
             </c:ext>
@@ -771,79 +781,79 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>39</c:v>
+                  <c:v>39.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>40.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41</c:v>
+                  <c:v>41.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42</c:v>
+                  <c:v>42.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43</c:v>
+                  <c:v>43.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44</c:v>
+                  <c:v>44.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>45</c:v>
+                  <c:v>45.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>46</c:v>
+                  <c:v>46.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>47</c:v>
+                  <c:v>47.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>48</c:v>
+                  <c:v>48.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>49</c:v>
+                  <c:v>49.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>50</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>51</c:v>
+                  <c:v>51.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>52</c:v>
+                  <c:v>52.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>9</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -855,85 +865,85 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43</c:v>
+                  <c:v>43.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>57</c:v>
+                  <c:v>57.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>83</c:v>
+                  <c:v>83.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>92</c:v>
+                  <c:v>92.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>96</c:v>
+                  <c:v>96.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>108</c:v>
+                  <c:v>108.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>133</c:v>
+                  <c:v>133.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>133</c:v>
+                  <c:v>133.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>133</c:v>
+                  <c:v>133.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>133</c:v>
+                  <c:v>133.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>133</c:v>
+                  <c:v>133.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>133</c:v>
+                  <c:v>133.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>133</c:v>
+                  <c:v>133.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>133</c:v>
+                  <c:v>133.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>133</c:v>
+                  <c:v>133.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>133</c:v>
+                  <c:v>133.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>133</c:v>
+                  <c:v>133.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>133</c:v>
+                  <c:v>133.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>133</c:v>
+                  <c:v>133.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>133</c:v>
+                  <c:v>133.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>133</c:v>
+                  <c:v>133.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>133</c:v>
+                  <c:v>133.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-8D59-4CCE-98CB-8B5DAB46F197}"/>
             </c:ext>
@@ -948,11 +958,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1361838784"/>
-        <c:axId val="-1359568384"/>
+        <c:axId val="-621171200"/>
+        <c:axId val="-621167040"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1361838784"/>
+        <c:axId val="-621171200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -984,6 +994,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1050,7 +1061,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1359568384"/>
+        <c:crossAx val="-621167040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1058,7 +1069,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1359568384"/>
+        <c:axId val="-621167040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1104,6 +1115,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1164,7 +1176,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1361838784"/>
+        <c:crossAx val="-621171200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1178,6 +1190,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1245,9 +1258,9 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="de-CH"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1289,6 +1302,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1349,79 +1363,79 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>39</c:v>
+                  <c:v>39.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>40.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41</c:v>
+                  <c:v>41.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42</c:v>
+                  <c:v>42.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43</c:v>
+                  <c:v>43.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44</c:v>
+                  <c:v>44.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>45</c:v>
+                  <c:v>45.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>46</c:v>
+                  <c:v>46.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>47</c:v>
+                  <c:v>47.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>48</c:v>
+                  <c:v>48.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>49</c:v>
+                  <c:v>49.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>50</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>51</c:v>
+                  <c:v>51.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>52</c:v>
+                  <c:v>52.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>9</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1433,85 +1447,85 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40</c:v>
+                  <c:v>40.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>56</c:v>
+                  <c:v>56.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>72</c:v>
+                  <c:v>72.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>88</c:v>
+                  <c:v>88.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>104</c:v>
+                  <c:v>104.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>120</c:v>
+                  <c:v>120.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>136</c:v>
+                  <c:v>136.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>152</c:v>
+                  <c:v>152.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>168</c:v>
+                  <c:v>168.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>184</c:v>
+                  <c:v>184.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>200</c:v>
+                  <c:v>200.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>200</c:v>
+                  <c:v>200.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>200</c:v>
+                  <c:v>200.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>216</c:v>
+                  <c:v>216.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>232</c:v>
+                  <c:v>232.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>248</c:v>
+                  <c:v>248.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>264</c:v>
+                  <c:v>264.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>280</c:v>
+                  <c:v>280.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>296</c:v>
+                  <c:v>296.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>312</c:v>
+                  <c:v>312.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>328</c:v>
+                  <c:v>328.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>344</c:v>
+                  <c:v>344.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>360</c:v>
+                  <c:v>360.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-89D9-4C5C-9F7A-65F21CAB559C}"/>
             </c:ext>
@@ -1542,79 +1556,79 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>39</c:v>
+                  <c:v>39.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>40.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41</c:v>
+                  <c:v>41.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42</c:v>
+                  <c:v>42.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43</c:v>
+                  <c:v>43.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44</c:v>
+                  <c:v>44.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>45</c:v>
+                  <c:v>45.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>46</c:v>
+                  <c:v>46.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>47</c:v>
+                  <c:v>47.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>48</c:v>
+                  <c:v>48.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>49</c:v>
+                  <c:v>49.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>50</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>51</c:v>
+                  <c:v>51.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>52</c:v>
+                  <c:v>52.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>9</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1626,85 +1640,85 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29</c:v>
+                  <c:v>29.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40</c:v>
+                  <c:v>40.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43</c:v>
+                  <c:v>43.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>57</c:v>
+                  <c:v>57.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>69</c:v>
+                  <c:v>69.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>79</c:v>
+                  <c:v>79.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>86</c:v>
+                  <c:v>86.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>111</c:v>
+                  <c:v>111.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>126</c:v>
+                  <c:v>126.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>133</c:v>
+                  <c:v>133.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>142</c:v>
+                  <c:v>142.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>169</c:v>
+                  <c:v>169.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>169</c:v>
+                  <c:v>173.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>169</c:v>
+                  <c:v>179.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>169</c:v>
+                  <c:v>179.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>169</c:v>
+                  <c:v>179.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>169</c:v>
+                  <c:v>179.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>169</c:v>
+                  <c:v>179.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>169</c:v>
+                  <c:v>179.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>169</c:v>
+                  <c:v>179.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>169</c:v>
+                  <c:v>179.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>169</c:v>
+                  <c:v>179.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>169</c:v>
+                  <c:v>179.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>169</c:v>
+                  <c:v>179.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-89D9-4C5C-9F7A-65F21CAB559C}"/>
             </c:ext>
@@ -1719,11 +1733,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1377989776"/>
-        <c:axId val="-1377981504"/>
+        <c:axId val="-624024112"/>
+        <c:axId val="-624020720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1377989776"/>
+        <c:axId val="-624024112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1755,6 +1769,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1821,7 +1836,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1377981504"/>
+        <c:crossAx val="-624020720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1829,7 +1844,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1377981504"/>
+        <c:axId val="-624020720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1875,6 +1890,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1935,7 +1951,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1377989776"/>
+        <c:crossAx val="-624024112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1949,6 +1965,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3463,23 +3480,23 @@
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.875" customWidth="1"/>
-    <col min="2" max="2" width="11.625" customWidth="1"/>
-    <col min="3" max="3" width="11.125" customWidth="1"/>
-    <col min="7" max="7" width="4.625" customWidth="1"/>
-    <col min="8" max="8" width="4.875" customWidth="1"/>
-    <col min="11" max="11" width="13.875" customWidth="1"/>
-    <col min="13" max="13" width="12.875" customWidth="1"/>
+    <col min="1" max="1" width="11.83203125" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" customWidth="1"/>
+    <col min="7" max="7" width="4.6640625" customWidth="1"/>
+    <col min="8" max="8" width="4.83203125" customWidth="1"/>
+    <col min="11" max="11" width="13.83203125" customWidth="1"/>
+    <col min="13" max="13" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="11" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="11" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>21</v>
       </c>
@@ -3487,7 +3504,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
@@ -3507,33 +3524,33 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="e">
         <f ca="1">VLOOKUP(Zusatz!J2,Zusatz!A2:C26,3)</f>
-        <v>360</v>
+        <v>#N/A</v>
       </c>
       <c r="B5" s="7">
         <f>'Raphael Bolliger'!C45</f>
         <v>133</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="7" t="e">
         <f ca="1">B5-A5</f>
-        <v>-227</v>
-      </c>
-      <c r="I5" s="7">
+        <v>#N/A</v>
+      </c>
+      <c r="I5" s="7" t="e">
         <f ca="1">VLOOKUP(Zusatz!J2,Zusatz!A2:C26,3)</f>
-        <v>360</v>
+        <v>#N/A</v>
       </c>
       <c r="J5" s="7">
         <f>'Andreas Lüscher'!C43</f>
-        <v>169</v>
-      </c>
-      <c r="K5" s="7">
+        <v>179</v>
+      </c>
+      <c r="K5" s="7" t="e">
         <f ca="1">J5-I5</f>
-        <v>-191</v>
-      </c>
-    </row>
-    <row r="29" spans="13:15" x14ac:dyDescent="0.25">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="29" spans="13:15" x14ac:dyDescent="0.2">
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
       <c r="O29" s="7"/>
@@ -3552,22 +3569,22 @@
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" style="7" customWidth="1"/>
     <col min="3" max="3" width="13" style="7" customWidth="1"/>
-    <col min="4" max="4" width="23.375" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" customWidth="1"/>
     <col min="5" max="5" width="50.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="11" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="11" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
     </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>18</v>
       </c>
@@ -3584,7 +3601,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <f>WEEKNUM(B4)</f>
         <v>39</v>
@@ -3602,7 +3619,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <f t="shared" ref="A5:A44" si="0">WEEKNUM(B5)</f>
         <v>40</v>
@@ -3620,7 +3637,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -3638,7 +3655,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -3653,7 +3670,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -3671,7 +3688,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -3689,7 +3706,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -3707,7 +3724,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -3722,7 +3739,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -3740,7 +3757,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -3758,7 +3775,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -3776,7 +3793,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -3794,7 +3811,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -3812,7 +3829,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -3830,7 +3847,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -3848,7 +3865,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -3866,7 +3883,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -3884,7 +3901,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -3902,7 +3919,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -3920,7 +3937,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -3938,7 +3955,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -3956,7 +3973,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="7">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -3974,7 +3991,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="7">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -3992,7 +4009,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="7">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -4010,7 +4027,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="7">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -4028,7 +4045,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="7">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -4046,7 +4063,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4054,7 +4071,7 @@
       <c r="B30" s="5"/>
       <c r="C30" s="6"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4062,7 +4079,7 @@
       <c r="B31" s="5"/>
       <c r="C31" s="6"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4070,7 +4087,7 @@
       <c r="B32" s="5"/>
       <c r="C32" s="6"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4078,7 +4095,7 @@
       <c r="B33" s="5"/>
       <c r="C33" s="6"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4086,7 +4103,7 @@
       <c r="B34" s="5"/>
       <c r="C34" s="6"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4094,7 +4111,7 @@
       <c r="B35" s="5"/>
       <c r="C35" s="6"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4102,7 +4119,7 @@
       <c r="B36" s="5"/>
       <c r="C36" s="6"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4110,7 +4127,7 @@
       <c r="B37" s="5"/>
       <c r="C37" s="6"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4118,7 +4135,7 @@
       <c r="B38" s="5"/>
       <c r="C38" s="6"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4126,7 +4143,7 @@
       <c r="B39" s="5"/>
       <c r="C39" s="6"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4134,7 +4151,7 @@
       <c r="B40" s="5"/>
       <c r="C40" s="6"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4142,7 +4159,7 @@
       <c r="B41" s="5"/>
       <c r="C41" s="6"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4150,7 +4167,7 @@
       <c r="B42" s="5"/>
       <c r="C42" s="6"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4158,7 +4175,7 @@
       <c r="B43" s="5"/>
       <c r="C43" s="6"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4166,23 +4183,23 @@
       <c r="B44" s="5"/>
       <c r="C44" s="6"/>
     </row>
-    <row r="45" spans="1:3" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="B45" s="19"/>
       <c r="C45" s="20">
         <f>SUM(C4:C44)</f>
         <v>133</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B46" s="5"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B47" s="5"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B48" s="5"/>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B49" s="5"/>
     </row>
   </sheetData>
@@ -4195,24 +4212,24 @@
   <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="13" style="7" customWidth="1"/>
-    <col min="4" max="4" width="34.125" customWidth="1"/>
+    <col min="4" max="4" width="34.1640625" customWidth="1"/>
     <col min="5" max="5" width="50.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="11" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="11" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="18"/>
     </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>18</v>
       </c>
@@ -4229,7 +4246,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <f>WEEKNUM(B4)</f>
         <v>39</v>
@@ -4247,7 +4264,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <f t="shared" ref="A5:A7" si="0">WEEKNUM(B5)</f>
         <v>40</v>
@@ -4265,7 +4282,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -4283,7 +4300,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -4298,7 +4315,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <f>WEEKNUM(B8)</f>
         <v>40</v>
@@ -4316,7 +4333,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <f>WEEKNUM(B9)</f>
         <v>41</v>
@@ -4334,7 +4351,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <f>WEEKNUM(B10)</f>
         <v>41</v>
@@ -4352,7 +4369,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <f>WEEKNUM(B11)</f>
         <v>42</v>
@@ -4367,7 +4384,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <f t="shared" ref="A12" si="1">WEEKNUM(B12)</f>
         <v>40</v>
@@ -4385,7 +4402,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <f>WEEKNUM(B13)</f>
         <v>43</v>
@@ -4403,7 +4420,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
         <f>WEEKNUM(B14)</f>
         <v>43</v>
@@ -4421,7 +4438,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
         <f>WEEKNUM(B15)</f>
         <v>44</v>
@@ -4439,7 +4456,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <f t="shared" ref="A16:A42" si="2">WEEKNUM(B16)</f>
         <v>44</v>
@@ -4457,7 +4474,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
         <v>44</v>
       </c>
@@ -4474,7 +4491,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
         <v>45</v>
       </c>
@@ -4491,7 +4508,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -4509,7 +4526,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -4527,7 +4544,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
         <f t="shared" si="2"/>
         <v>46</v>
@@ -4542,7 +4559,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
         <f t="shared" si="2"/>
         <v>46</v>
@@ -4560,7 +4577,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
         <f t="shared" si="2"/>
         <v>47</v>
@@ -4578,7 +4595,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
         <f t="shared" si="2"/>
         <v>47</v>
@@ -4596,7 +4613,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="7">
         <f t="shared" si="2"/>
         <v>47</v>
@@ -4614,7 +4631,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="7">
         <f t="shared" si="2"/>
         <v>47</v>
@@ -4632,7 +4649,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="7">
         <f t="shared" si="2"/>
         <v>48</v>
@@ -4650,7 +4667,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="7">
         <f t="shared" si="2"/>
         <v>48</v>
@@ -4668,7 +4685,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="7">
         <f t="shared" si="2"/>
         <v>48</v>
@@ -4686,7 +4703,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="7">
         <f t="shared" si="2"/>
         <v>49</v>
@@ -4704,7 +4721,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="7">
         <f t="shared" si="2"/>
         <v>49</v>
@@ -4722,7 +4739,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="7">
         <f t="shared" si="2"/>
         <v>50</v>
@@ -4740,7 +4757,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="7">
         <f t="shared" si="2"/>
         <v>50</v>
@@ -4758,7 +4775,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="7">
         <f t="shared" si="2"/>
         <v>51</v>
@@ -4776,7 +4793,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="7">
         <f t="shared" si="2"/>
         <v>51</v>
@@ -4794,7 +4811,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="7">
         <f t="shared" si="2"/>
         <v>51</v>
@@ -4812,7 +4829,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="7">
         <f t="shared" si="2"/>
         <v>51</v>
@@ -4830,7 +4847,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="7">
         <f t="shared" ref="A38" si="3">WEEKNUM(B38)</f>
         <v>51</v>
@@ -4848,23 +4865,43 @@
         <v>86</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="B39" s="3"/>
-      <c r="C39" s="6"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="B39" s="5">
+        <v>42724</v>
+      </c>
+      <c r="C39" s="6">
+        <v>4</v>
+      </c>
+      <c r="D39" t="s">
+        <v>91</v>
+      </c>
+      <c r="E39" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="B40" s="3"/>
-      <c r="C40" s="6"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="B40" s="5">
+        <v>42738</v>
+      </c>
+      <c r="C40" s="6">
+        <v>6</v>
+      </c>
+      <c r="D40" t="s">
+        <v>91</v>
+      </c>
+      <c r="E40" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="7">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4872,7 +4909,7 @@
       <c r="B41" s="3"/>
       <c r="C41" s="6"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="7">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4880,23 +4917,23 @@
       <c r="B42" s="3"/>
       <c r="C42" s="6"/>
     </row>
-    <row r="43" spans="1:5" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="B43" s="8"/>
       <c r="C43" s="20">
         <f>SUM(C4:C42)</f>
-        <v>169</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B44" s="3"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B45" s="3"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B46" s="3"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B47" s="3"/>
     </row>
   </sheetData>
@@ -4912,9 +4949,9 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="11.875" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4978,11 +5015,11 @@
       <c r="H2" s="17"/>
       <c r="I2" s="16">
         <f ca="1">TODAY()</f>
-        <v>42722</v>
+        <v>42738</v>
       </c>
       <c r="J2" s="17">
         <f ca="1">WEEKNUM(I2)</f>
-        <v>52</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -5378,11 +5415,11 @@
       </c>
       <c r="F15" s="17">
         <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$42,A15,'Andreas Lüscher'!$C$4:$C$42)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G15" s="17">
         <f ca="1">SUM(F$2:F15)</f>
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H15" s="17"/>
       <c r="I15" s="17"/>
@@ -5409,11 +5446,11 @@
       </c>
       <c r="F16" s="17">
         <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$42,A16,'Andreas Lüscher'!$C$4:$C$42)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G16" s="17">
         <f ca="1">SUM(F$2:F16)</f>
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="H16" s="17"/>
       <c r="I16" s="17"/>
@@ -5444,7 +5481,7 @@
       </c>
       <c r="G17" s="17">
         <f ca="1">SUM(F$2:F17)</f>
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="H17" s="17"/>
       <c r="I17" s="17"/>
@@ -5475,7 +5512,7 @@
       </c>
       <c r="G18" s="17">
         <f ca="1">SUM(F$2:F18)</f>
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="H18" s="17"/>
       <c r="I18" s="17"/>
@@ -5506,7 +5543,7 @@
       </c>
       <c r="G19" s="17">
         <f ca="1">SUM(F$2:F19)</f>
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="H19" s="17"/>
       <c r="I19" s="17"/>
@@ -5537,7 +5574,7 @@
       </c>
       <c r="G20" s="17">
         <f ca="1">SUM(F$2:F20)</f>
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="H20" s="17"/>
       <c r="I20" s="17"/>
@@ -5568,7 +5605,7 @@
       </c>
       <c r="G21" s="17">
         <f ca="1">SUM(F$2:F21)</f>
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="H21" s="17"/>
       <c r="I21" s="17"/>
@@ -5599,7 +5636,7 @@
       </c>
       <c r="G22" s="17">
         <f ca="1">SUM(F$2:F22)</f>
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="H22" s="17"/>
       <c r="I22" s="17"/>
@@ -5630,7 +5667,7 @@
       </c>
       <c r="G23" s="17">
         <f ca="1">SUM(F$2:F23)</f>
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="H23" s="17"/>
       <c r="I23" s="17"/>
@@ -5661,7 +5698,7 @@
       </c>
       <c r="G24" s="17">
         <f ca="1">SUM(F$2:F24)</f>
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="H24" s="17"/>
       <c r="I24" s="17"/>
@@ -5692,7 +5729,7 @@
       </c>
       <c r="G25" s="17">
         <f ca="1">SUM(F$2:F25)</f>
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="H25" s="17"/>
       <c r="I25" s="17"/>
@@ -5723,7 +5760,7 @@
       </c>
       <c r="G26" s="17">
         <f ca="1">SUM(F$2:F26)</f>
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="H26" s="17"/>
       <c r="I26" s="17"/>

</xml_diff>

<commit_message>
- documentation - updated journal
</commit_message>
<xml_diff>
--- a/doc/journal/Arbeitsjournal.xlsx
+++ b/doc/journal/Arbeitsjournal.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Daten/Spektrometer/portableSpectrometer/doc/journal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Andreas/Projects/Bachelorthesis/portableSpectrometer/doc/journal/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="49560" windowHeight="24720" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19700" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Arbeitsjournal" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="179">
   <si>
     <t>Arbeitsjournal Übersicht</t>
   </si>
@@ -492,6 +492,81 @@
   </si>
   <si>
     <t>Dokumentation</t>
+  </si>
+  <si>
+    <t>Writer erweitert und neu strukturiert</t>
+  </si>
+  <si>
+    <t>Unit Test mit Daten des Spektrometers erstellt und Writer verbessert</t>
+  </si>
+  <si>
+    <t>Unit Tests</t>
+  </si>
+  <si>
+    <t>Writer</t>
+  </si>
+  <si>
+    <t>Settings Modals verbessert und Radiance View Controller geändert</t>
+  </si>
+  <si>
+    <t>Spektras werden im Parent VC zwischengespeichert. Erst im Finish VC wird geschrieben.</t>
+  </si>
+  <si>
+    <t>UI &amp; Controller</t>
+  </si>
+  <si>
+    <t>RawSettings VC hinzugegfügt</t>
+  </si>
+  <si>
+    <t>Alle 3 Modi werden korrekt geschrieben</t>
+  </si>
+  <si>
+    <t>Refactoring</t>
+  </si>
+  <si>
+    <t>Calculations</t>
+  </si>
+  <si>
+    <t>Neue Calculations Klasse hinzugefügt und Command Manager verbessert</t>
+  </si>
+  <si>
+    <t>Radiance wird korrekt geschrieben inklusive base lamp und fo files</t>
+  </si>
+  <si>
+    <t>BackgroundFileManger</t>
+  </si>
+  <si>
+    <t>Neue BackgroundFileMangaer Klasse hinzugefügt, um Daten bereits während dem Messen zu schreiben.</t>
+  </si>
+  <si>
+    <t>FileSelection</t>
+  </si>
+  <si>
+    <t>Besuchte Pfade speichern und direkt dahinspringen, wenn FIleBrowser geöfnet wird.</t>
+  </si>
+  <si>
+    <t>File Managment</t>
+  </si>
+  <si>
+    <t>Verbessertes FileManagement</t>
+  </si>
+  <si>
+    <t>Instrument Control</t>
+  </si>
+  <si>
+    <t>Instument Control Aktionen hinzugefügt</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>Dokumentation erweitert</t>
+  </si>
+  <si>
+    <t>Page Classes hinzugefügt für die einfachere verwaltung der Parameter</t>
+  </si>
+  <si>
+    <t>Verbesserte Calculations, Writes und Anzeige der Messresultate. Grosses refactoring der Messmethoden</t>
   </si>
 </sst>
 </file>
@@ -1138,11 +1213,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-252960432"/>
-        <c:axId val="-123994272"/>
+        <c:axId val="1675858080"/>
+        <c:axId val="1675862112"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-252960432"/>
+        <c:axId val="1675858080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1241,7 +1316,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-123994272"/>
+        <c:crossAx val="1675862112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1249,7 +1324,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-123994272"/>
+        <c:axId val="1675862112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1356,7 +1431,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-252960432"/>
+        <c:crossAx val="1675858080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1877,22 +1952,22 @@
                   <c:v>249.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>249.0</c:v>
+                  <c:v>263.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>249.0</c:v>
+                  <c:v>287.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>249.0</c:v>
+                  <c:v>301.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>249.0</c:v>
+                  <c:v>342.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>249.0</c:v>
+                  <c:v>356.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>249.0</c:v>
+                  <c:v>356.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1913,11 +1988,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-153440592"/>
-        <c:axId val="-253121520"/>
+        <c:axId val="1675876624"/>
+        <c:axId val="1675880016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-153440592"/>
+        <c:axId val="1675876624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2016,7 +2091,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-253121520"/>
+        <c:crossAx val="1675880016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2024,7 +2099,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-253121520"/>
+        <c:axId val="1675880016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2131,7 +2206,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-153440592"/>
+        <c:crossAx val="1675876624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3657,7 +3732,7 @@
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3722,8 +3797,8 @@
         <v>#N/A</v>
       </c>
       <c r="J5" s="7">
-        <f>'Andreas Lüscher'!C58</f>
-        <v>249</v>
+        <f>'Andreas Lüscher'!C74</f>
+        <v>356</v>
       </c>
       <c r="K5" s="7" t="e">
         <f ca="1">J5-I5</f>
@@ -3745,7 +3820,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+    <sheetView topLeftCell="A36" workbookViewId="0">
       <selection activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
@@ -4993,10 +5068,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5723,7 +5798,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="7">
-        <f t="shared" ref="A43:A57" si="4">WEEKNUM(B43)</f>
+        <f t="shared" ref="A43:A73" si="4">WEEKNUM(B43)</f>
         <v>2</v>
       </c>
       <c r="B43" s="5">
@@ -5841,7 +5916,7 @@
         <v>3</v>
       </c>
       <c r="D49" t="s">
-        <v>91</v>
+        <v>163</v>
       </c>
       <c r="E49" t="s">
         <v>100</v>
@@ -5903,61 +5978,358 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="B53" s="5"/>
-      <c r="C53" s="6"/>
+        <f>WEEKNUM(B53)</f>
+        <v>6</v>
+      </c>
+      <c r="B53" s="5">
+        <v>42773</v>
+      </c>
+      <c r="C53" s="6">
+        <v>6</v>
+      </c>
+      <c r="D53" t="s">
+        <v>157</v>
+      </c>
+      <c r="E53" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="B54" s="5"/>
-      <c r="C54" s="6"/>
+        <v>6</v>
+      </c>
+      <c r="B54" s="5">
+        <v>42775</v>
+      </c>
+      <c r="C54" s="6">
+        <v>8</v>
+      </c>
+      <c r="D54" t="s">
+        <v>156</v>
+      </c>
+      <c r="E54" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="B55" s="5"/>
-      <c r="C55" s="6"/>
+        <v>7</v>
+      </c>
+      <c r="B55" s="5">
+        <v>42780</v>
+      </c>
+      <c r="C55" s="6">
+        <v>7</v>
+      </c>
+      <c r="D55" t="s">
+        <v>71</v>
+      </c>
+      <c r="E55" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="B56" s="5"/>
-      <c r="C56" s="6"/>
+        <v>7</v>
+      </c>
+      <c r="B56" s="5">
+        <v>42781</v>
+      </c>
+      <c r="C56" s="6">
+        <v>7</v>
+      </c>
+      <c r="D56" t="s">
+        <v>105</v>
+      </c>
+      <c r="E56" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="7">
         <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="B57" s="5">
+        <v>42782</v>
+      </c>
+      <c r="C57" s="6">
+        <v>5</v>
+      </c>
+      <c r="D57" t="s">
+        <v>105</v>
+      </c>
+      <c r="E57" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" s="7">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="B58" s="5">
+        <v>42783</v>
+      </c>
+      <c r="C58" s="6">
+        <v>5</v>
+      </c>
+      <c r="D58" t="s">
+        <v>160</v>
+      </c>
+      <c r="E58" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" s="7">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="B59" s="5">
+        <v>42786</v>
+      </c>
+      <c r="C59" s="6">
+        <v>4</v>
+      </c>
+      <c r="D59" t="s">
+        <v>157</v>
+      </c>
+      <c r="E59" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" s="7">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="B60" s="5">
+        <v>42790</v>
+      </c>
+      <c r="C60" s="6">
+        <v>6</v>
+      </c>
+      <c r="D60" t="s">
+        <v>163</v>
+      </c>
+      <c r="E60" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" s="7">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="B61" s="5">
+        <v>42791</v>
+      </c>
+      <c r="C61" s="6">
+        <v>4</v>
+      </c>
+      <c r="D61" t="s">
+        <v>164</v>
+      </c>
+      <c r="E61" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" s="7">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="B62" s="5">
+        <v>42792</v>
+      </c>
+      <c r="C62" s="6">
+        <v>4</v>
+      </c>
+      <c r="D62" t="s">
+        <v>157</v>
+      </c>
+      <c r="E62" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" s="7">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="B63" s="5">
+        <v>42794</v>
+      </c>
+      <c r="C63" s="6">
+        <v>9</v>
+      </c>
+      <c r="D63" t="s">
+        <v>167</v>
+      </c>
+      <c r="E63" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" s="7">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="B64" s="5">
+        <v>42795</v>
+      </c>
+      <c r="C64" s="6">
+        <v>12</v>
+      </c>
+      <c r="D64" t="s">
+        <v>105</v>
+      </c>
+      <c r="E64" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" s="7">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="B65" s="5">
+        <v>42796</v>
+      </c>
+      <c r="C65" s="6">
+        <v>7</v>
+      </c>
+      <c r="D65" t="s">
+        <v>169</v>
+      </c>
+      <c r="E65" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" s="7">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="B66" s="5">
+        <v>42796</v>
+      </c>
+      <c r="C66" s="6">
+        <v>4</v>
+      </c>
+      <c r="D66" t="s">
+        <v>171</v>
+      </c>
+      <c r="E66" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" s="7">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="B67" s="5">
+        <v>42797</v>
+      </c>
+      <c r="C67" s="6">
+        <v>5</v>
+      </c>
+      <c r="D67" t="s">
+        <v>173</v>
+      </c>
+      <c r="E67" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" s="7">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="B68" s="5">
+        <v>42800</v>
+      </c>
+      <c r="C68" s="6">
+        <v>8</v>
+      </c>
+      <c r="D68" t="s">
+        <v>175</v>
+      </c>
+      <c r="E68" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" s="7">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="B69" s="5">
+        <v>42801</v>
+      </c>
+      <c r="C69" s="6">
+        <v>6</v>
+      </c>
+      <c r="D69" t="s">
+        <v>175</v>
+      </c>
+      <c r="E69" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" s="7">
+        <f t="shared" ref="A70" si="5">WEEKNUM(B70)</f>
         <v>0</v>
       </c>
-      <c r="B57" s="5"/>
-    </row>
-    <row r="58" spans="1:5" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="B58" s="8"/>
-      <c r="C58" s="20">
-        <f>SUM(C4:C56)</f>
-        <v>249</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B59" s="3"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B60" s="3"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B61" s="3"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B62" s="3"/>
+      <c r="B70" s="5"/>
+      <c r="C70" s="6"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="B71" s="5"/>
+      <c r="C71" s="6"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" s="7">
+        <f t="shared" ref="A72" si="6">WEEKNUM(B72)</f>
+        <v>0</v>
+      </c>
+      <c r="B72" s="5"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="B73" s="5"/>
+    </row>
+    <row r="74" spans="1:5" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="B74" s="8"/>
+      <c r="C74" s="20">
+        <f>SUM(C4:C72)</f>
+        <v>356</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B75" s="3"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B76" s="3"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B77" s="3"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B78" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6028,7 +6400,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="17">
-        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$56,A2,'Andreas Lüscher'!$C$4:$C$56)</f>
+        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$72,A2,'Andreas Lüscher'!$C$4:$C$72)</f>
         <v>3</v>
       </c>
       <c r="G2" s="17">
@@ -6038,7 +6410,7 @@
       <c r="H2" s="17"/>
       <c r="I2" s="16">
         <f ca="1">TODAY()</f>
-        <v>42801</v>
+        <v>42802</v>
       </c>
       <c r="J2" s="17">
         <f ca="1">WEEKNUM(I2)</f>
@@ -6065,7 +6437,7 @@
         <v>20</v>
       </c>
       <c r="F3" s="17">
-        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$56,A3,'Andreas Lüscher'!$C$4:$C$56)</f>
+        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$72,A3,'Andreas Lüscher'!$C$4:$C$72)</f>
         <v>26</v>
       </c>
       <c r="G3" s="17">
@@ -6096,7 +6468,7 @@
         <v>32</v>
       </c>
       <c r="F4" s="17">
-        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$56,A4,'Andreas Lüscher'!$C$4:$C$56)</f>
+        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$72,A4,'Andreas Lüscher'!$C$4:$C$72)</f>
         <v>11</v>
       </c>
       <c r="G4" s="17">
@@ -6127,7 +6499,7 @@
         <v>43</v>
       </c>
       <c r="F5" s="17">
-        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$56,A5,'Andreas Lüscher'!$C$4:$C$56)</f>
+        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$72,A5,'Andreas Lüscher'!$C$4:$C$72)</f>
         <v>3</v>
       </c>
       <c r="G5" s="17">
@@ -6158,7 +6530,7 @@
         <v>57</v>
       </c>
       <c r="F6" s="17">
-        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$56,A6,'Andreas Lüscher'!$C$4:$C$56)</f>
+        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$72,A6,'Andreas Lüscher'!$C$4:$C$72)</f>
         <v>14</v>
       </c>
       <c r="G6" s="17">
@@ -6189,7 +6561,7 @@
         <v>83</v>
       </c>
       <c r="F7" s="17">
-        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$56,A7,'Andreas Lüscher'!$C$4:$C$56)</f>
+        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$72,A7,'Andreas Lüscher'!$C$4:$C$72)</f>
         <v>12</v>
       </c>
       <c r="G7" s="17">
@@ -6220,7 +6592,7 @@
         <v>92</v>
       </c>
       <c r="F8" s="17">
-        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$56,A8,'Andreas Lüscher'!$C$4:$C$56)</f>
+        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$72,A8,'Andreas Lüscher'!$C$4:$C$72)</f>
         <v>10</v>
       </c>
       <c r="G8" s="17">
@@ -6251,7 +6623,7 @@
         <v>96</v>
       </c>
       <c r="F9" s="17">
-        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$56,A9,'Andreas Lüscher'!$C$4:$C$56)</f>
+        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$72,A9,'Andreas Lüscher'!$C$4:$C$72)</f>
         <v>7</v>
       </c>
       <c r="G9" s="17">
@@ -6282,7 +6654,7 @@
         <v>108</v>
       </c>
       <c r="F10" s="17">
-        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$56,A10,'Andreas Lüscher'!$C$4:$C$56)</f>
+        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$72,A10,'Andreas Lüscher'!$C$4:$C$72)</f>
         <v>25</v>
       </c>
       <c r="G10" s="17">
@@ -6313,7 +6685,7 @@
         <v>133</v>
       </c>
       <c r="F11" s="17">
-        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$56,A11,'Andreas Lüscher'!$C$4:$C$56)</f>
+        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$72,A11,'Andreas Lüscher'!$C$4:$C$72)</f>
         <v>15</v>
       </c>
       <c r="G11" s="17">
@@ -6344,7 +6716,7 @@
         <v>157</v>
       </c>
       <c r="F12" s="17">
-        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$56,A12,'Andreas Lüscher'!$C$4:$C$56)</f>
+        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$72,A12,'Andreas Lüscher'!$C$4:$C$72)</f>
         <v>7</v>
       </c>
       <c r="G12" s="17">
@@ -6375,7 +6747,7 @@
         <v>174</v>
       </c>
       <c r="F13" s="17">
-        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$56,A13,'Andreas Lüscher'!$C$4:$C$56)</f>
+        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$72,A13,'Andreas Lüscher'!$C$4:$C$72)</f>
         <v>9</v>
       </c>
       <c r="G13" s="17">
@@ -6406,7 +6778,7 @@
         <v>187</v>
       </c>
       <c r="F14" s="17">
-        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$56,A14,'Andreas Lüscher'!$C$4:$C$56)</f>
+        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$72,A14,'Andreas Lüscher'!$C$4:$C$72)</f>
         <v>27</v>
       </c>
       <c r="G14" s="17">
@@ -6437,7 +6809,7 @@
         <v>195</v>
       </c>
       <c r="F15" s="17">
-        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$56,A15,'Andreas Lüscher'!$C$4:$C$56)</f>
+        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$72,A15,'Andreas Lüscher'!$C$4:$C$72)</f>
         <v>4</v>
       </c>
       <c r="G15" s="17">
@@ -6468,7 +6840,7 @@
         <v>195</v>
       </c>
       <c r="F16" s="17">
-        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$56,A16,'Andreas Lüscher'!$C$4:$C$56)</f>
+        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$72,A16,'Andreas Lüscher'!$C$4:$C$72)</f>
         <v>6</v>
       </c>
       <c r="G16" s="17">
@@ -6499,7 +6871,7 @@
         <v>195</v>
       </c>
       <c r="F17" s="17">
-        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$56,A17,'Andreas Lüscher'!$C$4:$C$56)</f>
+        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$72,A17,'Andreas Lüscher'!$C$4:$C$72)</f>
         <v>20</v>
       </c>
       <c r="G17" s="17">
@@ -6530,7 +6902,7 @@
         <v>196</v>
       </c>
       <c r="F18" s="17">
-        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$56,A18,'Andreas Lüscher'!$C$4:$C$56)</f>
+        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$72,A18,'Andreas Lüscher'!$C$4:$C$72)</f>
         <v>16</v>
       </c>
       <c r="G18" s="17">
@@ -6561,7 +6933,7 @@
         <v>220</v>
       </c>
       <c r="F19" s="17">
-        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$56,A19,'Andreas Lüscher'!$C$4:$C$56)</f>
+        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$72,A19,'Andreas Lüscher'!$C$4:$C$72)</f>
         <v>12</v>
       </c>
       <c r="G19" s="17">
@@ -6592,7 +6964,7 @@
         <v>238</v>
       </c>
       <c r="F20" s="17">
-        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$56,A20,'Andreas Lüscher'!$C$4:$C$56)</f>
+        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$72,A20,'Andreas Lüscher'!$C$4:$C$72)</f>
         <v>22</v>
       </c>
       <c r="G20" s="17">
@@ -6623,12 +6995,12 @@
         <v>257</v>
       </c>
       <c r="F21" s="17">
-        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$56,A21,'Andreas Lüscher'!$C$4:$C$56)</f>
-        <v>0</v>
+        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$72,A21,'Andreas Lüscher'!$C$4:$C$72)</f>
+        <v>14</v>
       </c>
       <c r="G21" s="17">
         <f ca="1">SUM(F$2:F21)</f>
-        <v>249</v>
+        <v>263</v>
       </c>
       <c r="H21" s="17"/>
       <c r="I21" s="17"/>
@@ -6654,12 +7026,12 @@
         <v>289</v>
       </c>
       <c r="F22" s="17">
-        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$56,A22,'Andreas Lüscher'!$C$4:$C$56)</f>
-        <v>0</v>
+        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$72,A22,'Andreas Lüscher'!$C$4:$C$72)</f>
+        <v>24</v>
       </c>
       <c r="G22" s="17">
         <f ca="1">SUM(F$2:F22)</f>
-        <v>249</v>
+        <v>287</v>
       </c>
       <c r="H22" s="17"/>
       <c r="I22" s="17"/>
@@ -6685,12 +7057,12 @@
         <v>333</v>
       </c>
       <c r="F23" s="17">
-        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$56,A23,'Andreas Lüscher'!$C$4:$C$56)</f>
-        <v>0</v>
+        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$72,A23,'Andreas Lüscher'!$C$4:$C$72)</f>
+        <v>14</v>
       </c>
       <c r="G23" s="17">
         <f ca="1">SUM(F$2:F23)</f>
-        <v>249</v>
+        <v>301</v>
       </c>
       <c r="H23" s="17"/>
       <c r="I23" s="17"/>
@@ -6716,12 +7088,12 @@
         <v>386</v>
       </c>
       <c r="F24" s="17">
-        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$56,A24,'Andreas Lüscher'!$C$4:$C$56)</f>
-        <v>0</v>
+        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$72,A24,'Andreas Lüscher'!$C$4:$C$72)</f>
+        <v>41</v>
       </c>
       <c r="G24" s="17">
         <f ca="1">SUM(F$2:F24)</f>
-        <v>249</v>
+        <v>342</v>
       </c>
       <c r="H24" s="17"/>
       <c r="I24" s="17"/>
@@ -6747,12 +7119,12 @@
         <v>404</v>
       </c>
       <c r="F25" s="17">
-        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$56,A25,'Andreas Lüscher'!$C$4:$C$56)</f>
-        <v>0</v>
+        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$72,A25,'Andreas Lüscher'!$C$4:$C$72)</f>
+        <v>14</v>
       </c>
       <c r="G25" s="17">
         <f ca="1">SUM(F$2:F25)</f>
-        <v>249</v>
+        <v>356</v>
       </c>
       <c r="H25" s="17"/>
       <c r="I25" s="17"/>
@@ -6778,12 +7150,12 @@
         <v>404</v>
       </c>
       <c r="F26" s="17">
-        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$56,A26,'Andreas Lüscher'!$C$4:$C$56)</f>
+        <f ca="1">SUMIF('Andreas Lüscher'!$A$4:$C$72,A26,'Andreas Lüscher'!$C$4:$C$72)</f>
         <v>0</v>
       </c>
       <c r="G26" s="17">
         <f ca="1">SUM(F$2:F26)</f>
-        <v>249</v>
+        <v>356</v>
       </c>
       <c r="H26" s="17"/>
       <c r="I26" s="17"/>

</xml_diff>